<commit_message>
Updated BOM for v2.1.
</commit_message>
<xml_diff>
--- a/oresat-backplane-bom.xlsx
+++ b/oresat-backplane-bom.xlsx
@@ -21,13 +21,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4" count="4">
   <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>Digi-Key</t>
   </si>
   <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>P</t>
   </si>
   <si>
     <t>Samtec</t>
@@ -113,7 +113,7 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -170,13 +170,21 @@
     <row r="3" spans="1:18" ht="13.5">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Last modified: 2018/10/02</t>
+          <t>PCB version: 2.1</t>
         </is>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>P/DNP = </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Place/Do Not Place (DNP is for final production boards)</t>
+        </is>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -186,19 +194,19 @@
     <row r="4" spans="1:18" ht="13.5">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>PCB version: 1.0</t>
+          <t>BOM revision: 0</t>
         </is>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>P/DNP = </t>
+          <t>Generic = </t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Place/Do Not Place (DNP is for final production boards)</t>
+          <t>Any generic part with the same characteristics are OK (e.g., bypass cap)</t>
         </is>
       </c>
       <c r="F4" s="2"/>
@@ -207,24 +215,12 @@
       <c r="I4" s="3"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:18" ht="13.5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>BOM revision: 0</t>
-        </is>
-      </c>
+    <row r="5" spans="1:18">
+      <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Generic = </t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Any generic part with the same characteristics are OK (e.g., bypass cap)</t>
-        </is>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -232,191 +228,269 @@
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:18">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Cnt</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Part References</t>
         </is>
       </c>
-      <c r="C7" s="3" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>P/DNP</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D6" s="2" t="inlineStr">
         <is>
           <t>Mfg</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="E6" s="2" t="inlineStr">
         <is>
           <t>Mfg PN</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="G7" s="2" t="inlineStr">
+      <c r="G6" s="2" t="inlineStr">
         <is>
           <t>Distributor</t>
         </is>
       </c>
-      <c r="H7" s="2" t="inlineStr">
+      <c r="H6" s="2" t="inlineStr">
         <is>
           <t>Dist. PN</t>
         </is>
       </c>
-      <c r="I7" s="3" t="inlineStr">
+      <c r="I6" s="3" t="inlineStr">
         <is>
           <t>Generic</t>
         </is>
       </c>
-      <c r="J7" s="2" t="inlineStr">
+      <c r="J6" s="2" t="inlineStr">
         <is>
           <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="13.5">
+      <c r="A7">
+        <v>10</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CM1.1, CM1.2, CM1.3, CM2.1, CM2.2, CM2.3, CM3.1, CM3.2, CM3.3, CM4.1, CM4.2, CM4.3, CM5.1, CM5.2, CM5.3, CM6.1, CM6.2, CM6.3, CM7.1, CM7.2, CM7.3, CM8.1, CM8.2, CM8.3, CM9.1, CM9.2, CM9.3, CM10.1, CM10.2, CM10.3, CM11.1, CM11.2, CM11.3, CM12.1, CM12.2, CM12.3, CM13.1, CM13.2, CM13.3, CM14.1, CM14.2, CM14.3, CM15.1, CM15.2, CM15.3, CM16.1, CM16.2, CM16.3, CM17.1, CM17.2, CM17.3, CM18.1, CM18.2, CM18.3, CM19.1, CM19.2, CM19.3, CM20.1, CM20.2, CM20.3</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Molex</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>073300-0110</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>SMPM Connector Plug, Male Pin 50 Ohm SMT + TH</t>
+        </is>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>WM10770-ND</t>
+        </is>
+      </c>
+      <c r="I7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Only 10 are ever stuffed</t>
         </is>
       </c>
     </row>
     <row r="8" spans="1:18" ht="13.5">
       <c r="A8">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CM1.1, CM1.2, CM1.3, CM2.1, CM2.2, CM2.3, CM3.1, CM3.2, CM3.3, CM4.1, CM4.2, CM4.3, CM5.1, CM5.2, CM5.3, CM6.1, CM6.2, CM6.3, CM7.1, CM7.2, CM7.3, CM8.1, CM8.2, CM8.3, CM9.1, CM9.2, CM9.3, CM10.1, CM10.2, CM10.3, CM11.1, CM11.2, CM11.3, CM12.1, CM12.2, CM12.3, CM13.1, CM13.2, CM13.3, CM14.1, CM14.2, CM14.3, CM15.1, CM15.2, CM15.3, CM16.1, CM16.2, CM16.3, CM17.1, CM17.2, CM17.3, CM18.1, CM18.2, CM18.3, CM19.1, CM19.2, CM19.3, CM20.1, CM20.2, CM20.3</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>DNP</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Molex</t>
-        </is>
+          <t>CF1.1, CF2.1, CF3.1, CF4.1, CF5.1, CF6.1, CF7.1, CF8.1, CF9.1, CF10.1, CF11.1, CF12.1, CF13.1, CF14.1, CF15.1, CF16.1, CF17.1, CF18.1, CF19.1, CF20.1</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>073300-0110</t>
+          <t>SFM-110-01-S-D-LC</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>SMPM Connector Plug, Male Pin 50 Ohm SMT + TH</t>
+          <t>TigerEye SFM series 20 pin 1.27 mm TH Vertical connector</t>
         </is>
       </c>
       <c r="G8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>WM10770-ND</t>
+          <t>SFM-110-01-S-D-LC-ND</t>
         </is>
       </c>
       <c r="I8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Do not populate except when necessary.</t>
+          <t>17 on board, but subtract 4 for batteries</t>
         </is>
       </c>
     </row>
     <row r="9" spans="1:18" ht="13.5">
       <c r="A9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CF1.1, CF2.1, CF3.1, CF4.1, CF5.1, CF6.1, CF7.1, CF8.1, CF9.1, CF10.1, CF11.1, CF12.1, CF13.1, CF14.1, CF15.1, CF16.1, CF17.1, CF18.1, CF19.1, CF20.1</t>
-        </is>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>2</v>
+          <t>CF2.2, CF3.2, CF4.2, CF5.2, CF6.2, CF7.2, CF8.2, CF9.2, CF10.2, CF11.2, CF12.2, CF13.2, CF14.2, CF15.2, CF16.2, CF17.2, CF18.2, CF19.2</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>DNP</t>
+        </is>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>SFM-110-01-S-D-LC</t>
+          <t>SFM-120-01-S-D-LC</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>TigerEye SFM series 20 pin 1.27 mm TH Vertical connector</t>
+          <t>TigerEye SFM series 40 pin 1.27 mm TH Vertical connector</t>
         </is>
       </c>
       <c r="G9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>SFM-110-01-S-D-LC-ND</t>
+          <t>SAM11706-ND</t>
         </is>
       </c>
       <c r="I9" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="13.5">
       <c r="A10">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CF2.2, CF3.2, CF4.2, CF5.2, CF6.2, CF7.2, CF8.2, CF9.2, CF10.2, CF11.2, CF12.2, CF13.2, CF14.2, CF15.2, CF16.2, CF17.2, CF18.2, CF19.2</t>
+          <t>R1, R2, R3, R4, R5, R6, R7, R8</t>
         </is>
       </c>
       <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Rohm</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ESR18EZPF60R4</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>60.4 Ohms ±1% 0.5W, 1/2W Resistor 1206 AEC-Q200</t>
+        </is>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>RHM60.4AFCT-ND</t>
+        </is>
+      </c>
+      <c r="I10" t="s">
         <v>2</v>
       </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>SFM-120-01-S-D-LC</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>TigerEye SFM series 40 pin 1.27 mm TH Vertical connector</t>
-        </is>
-      </c>
-      <c r="G10" t="s">
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>High wattage</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="13.5">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C1, C2, C3, C4</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>SAM11706-ND</t>
-        </is>
-      </c>
-      <c r="I10" t="s">
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Kemet</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>C0603C102F1GACAUTO</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>1000pF ±1% 100V Ceramic Capacitor C0G, NP0 0603</t>
+        </is>
+      </c>
+      <c r="G11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" ht="13.5">
-      <c r="C11" s="1"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>399-C0603C102F1GACAUTOCT-ND</t>
+        </is>
+      </c>
+      <c r="I11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>High voltage, automotive grade</t>
+        </is>
+      </c>
     </row>
     <row r="13" spans="1:18" ht="13.5">
       <c r="A13" t="inlineStr">
@@ -433,8 +507,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" ht="13.5">
-      <c r="A16">
-        <v>0</v>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1.0r0</t>
+        </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -442,7 +518,18 @@
         </is>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="13.5"/>
+    <row r="17" spans="1:18" ht="13.5">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2.1r0</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Added Rs and Cs, reduced SMPM connectors to the right number, cleaned up  for version 2.1r0.</t>
+        </is>
+      </c>
+    </row>
     <row r="1048559" spans="1:18">
       <c r="I1048559" s="0"/>
     </row>

</xml_diff>